<commit_message>
Changed MET level 20211 to MET level
</commit_message>
<xml_diff>
--- a/Lists/Job_list.xlsx
+++ b/Lists/Job_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coral\Documents\Universidad_2\Articulos\1. Articulo metodologia matlab code LTPAQ\LTPAQ_MATLAB_code\Lists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86DA06A6-60C9-4585-9722-75F644A1B8F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{154315A5-5517-46AB-9353-48FE384EA9C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5E1112A5-35B4-4BB2-957C-5EE8D223495B}"/>
   </bookViews>
@@ -432,9 +432,6 @@
     <t>Working out (as part of job, e.g., police)</t>
   </si>
   <si>
-    <t>MET Level 2011</t>
-  </si>
-  <si>
     <t>Walking, pushing or pulling stroller with child or walking with children, 2.5 to 3.1 mph</t>
   </si>
   <si>
@@ -445,6 +442,9 @@
   </si>
   <si>
     <t>Standing or lifting or kneeling or bending, (bartending, store clerk, filing, duplicating, librarian, xeroxing, assembling, hair dressing, standing and talking at work) light</t>
+  </si>
+  <si>
+    <t>MET Level</t>
   </si>
 </sst>
 </file>
@@ -859,7 +859,7 @@
   <dimension ref="A1:C132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="85.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -870,13 +870,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -1082,7 +1082,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C20" s="4">
         <v>2.5</v>
@@ -1940,7 +1940,7 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C98" s="4">
         <v>3</v>
@@ -2270,7 +2270,7 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C128" s="4">
         <v>4</v>

</xml_diff>